<commit_message>
3.0.14: Implement PermissionKindMap option to generate PermissionKindMap.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoVueComponentClassStructure.xlsx
+++ b/meta/program/BlancoVueComponentClassStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC83125E-A8D7-9E49-9FD1-AEEE8D4A7098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971314A9-4989-6F42-A8BB-0B26124EECBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2440" yWindow="7780" windowWidth="22500" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="129">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -799,6 +799,26 @@
     </rPh>
     <rPh sb="21" eb="23">
       <t xml:space="preserve">テイギシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>permissionKind</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>権限種別または権限グループでを表す文字列です。</t>
+    <rPh sb="0" eb="4">
+      <t xml:space="preserve">ケンゲンシュベツ </t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">ケンゲｎ </t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <rPh sb="17" eb="20">
+      <t xml:space="preserve">モジレツ </t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -1338,9 +1358,36 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1349,33 +1396,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1787,10 +1807,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1985,24 +2005,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="55"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="51"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="48"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="55"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="51"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -2044,30 +2064,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="52" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="23"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="48"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
       <c r="F26" s="8"/>
       <c r="G26"/>
     </row>
@@ -2108,7 +2128,7 @@
     </row>
     <row r="29" spans="1:7" ht="47" customHeight="1">
       <c r="A29" s="36">
-        <f t="shared" ref="A29:A64" si="0">A28+1</f>
+        <f t="shared" ref="A29:A65" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="37" t="s">
@@ -2118,10 +2138,10 @@
         <v>32</v>
       </c>
       <c r="D29" s="38"/>
-      <c r="E29" s="56" t="s">
+      <c r="E29" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="57"/>
+      <c r="F29" s="56"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="47" customHeight="1">
@@ -2136,10 +2156,10 @@
         <v>32</v>
       </c>
       <c r="D30" s="38"/>
-      <c r="E30" s="56" t="s">
+      <c r="E30" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="57"/>
+      <c r="F30" s="56"/>
       <c r="G30"/>
     </row>
     <row r="31" spans="1:7" ht="47" customHeight="1">
@@ -2154,10 +2174,10 @@
         <v>32</v>
       </c>
       <c r="D31" s="38"/>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="57"/>
+      <c r="F31" s="56"/>
       <c r="G31"/>
     </row>
     <row r="32" spans="1:7" ht="47" customHeight="1">
@@ -2172,10 +2192,10 @@
         <v>32</v>
       </c>
       <c r="D32" s="38"/>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="56"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="47" customHeight="1">
@@ -2190,10 +2210,10 @@
         <v>32</v>
       </c>
       <c r="D33" s="38"/>
-      <c r="E33" s="56" t="s">
+      <c r="E33" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="F33" s="57"/>
+      <c r="F33" s="56"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="15">
@@ -2231,7 +2251,7 @@
       <c r="E35" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="F35" s="51"/>
+      <c r="F35" s="47"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" ht="15">
@@ -2248,10 +2268,10 @@
       <c r="D36" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="52" t="s">
+      <c r="E36" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="F36" s="53"/>
+      <c r="F36" s="54"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="15">
@@ -2268,10 +2288,10 @@
       <c r="D37" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="52" t="s">
+      <c r="E37" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="F37" s="53"/>
+      <c r="F37" s="54"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" ht="15">
@@ -2288,10 +2308,10 @@
       <c r="D38" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="52" t="s">
+      <c r="E38" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="F38" s="53"/>
+      <c r="F38" s="54"/>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" ht="15">
@@ -2308,10 +2328,10 @@
       <c r="D39" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E39" s="52" t="s">
+      <c r="E39" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="F39" s="53"/>
+      <c r="F39" s="54"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="15">
@@ -2331,7 +2351,7 @@
       <c r="E40" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="F40" s="51"/>
+      <c r="F40" s="47"/>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7" ht="15">
@@ -2351,7 +2371,7 @@
       <c r="E41" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="F41" s="51"/>
+      <c r="F41" s="47"/>
       <c r="G41"/>
     </row>
     <row r="42" spans="1:7" ht="15">
@@ -2371,7 +2391,7 @@
       <c r="E42" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F42" s="51"/>
+      <c r="F42" s="47"/>
       <c r="G42"/>
     </row>
     <row r="43" spans="1:7" ht="15">
@@ -2391,7 +2411,7 @@
       <c r="E43" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="51"/>
+      <c r="F43" s="47"/>
       <c r="G43"/>
     </row>
     <row r="44" spans="1:7" ht="15">
@@ -2411,7 +2431,7 @@
       <c r="E44" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="F44" s="51"/>
+      <c r="F44" s="47"/>
       <c r="G44"/>
     </row>
     <row r="45" spans="1:7" ht="15">
@@ -2431,7 +2451,7 @@
       <c r="E45" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="F45" s="51"/>
+      <c r="F45" s="47"/>
       <c r="G45"/>
     </row>
     <row r="46" spans="1:7" ht="15">
@@ -2451,7 +2471,7 @@
       <c r="E46" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="F46" s="51"/>
+      <c r="F46" s="47"/>
       <c r="G46"/>
     </row>
     <row r="47" spans="1:7" ht="15">
@@ -2471,7 +2491,7 @@
       <c r="E47" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="F47" s="51"/>
+      <c r="F47" s="47"/>
       <c r="G47"/>
     </row>
     <row r="48" spans="1:7" ht="15">
@@ -2491,7 +2511,7 @@
       <c r="E48" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="F48" s="51"/>
+      <c r="F48" s="47"/>
       <c r="G48"/>
     </row>
     <row r="49" spans="1:7" ht="15">
@@ -2509,7 +2529,7 @@
       <c r="E49" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="F49" s="51"/>
+      <c r="F49" s="47"/>
       <c r="G49"/>
     </row>
     <row r="50" spans="1:7" ht="45" customHeight="1">
@@ -2529,7 +2549,7 @@
       <c r="E50" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="F50" s="47"/>
+      <c r="F50" s="50"/>
       <c r="G50"/>
     </row>
     <row r="51" spans="1:7" ht="45">
@@ -2549,7 +2569,7 @@
       <c r="E51" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="F51" s="47"/>
+      <c r="F51" s="50"/>
       <c r="G51"/>
     </row>
     <row r="52" spans="1:7" ht="45">
@@ -2569,7 +2589,7 @@
       <c r="E52" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="F52" s="47"/>
+      <c r="F52" s="50"/>
       <c r="G52"/>
     </row>
     <row r="53" spans="1:7" ht="45">
@@ -2589,7 +2609,7 @@
       <c r="E53" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="F53" s="47"/>
+      <c r="F53" s="50"/>
       <c r="G53"/>
     </row>
     <row r="54" spans="1:7" ht="15">
@@ -2607,7 +2627,7 @@
       <c r="E54" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="F54" s="47"/>
+      <c r="F54" s="50"/>
       <c r="G54"/>
     </row>
     <row r="55" spans="1:7">
@@ -2627,7 +2647,7 @@
       <c r="E55" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F55" s="51"/>
+      <c r="F55" s="47"/>
       <c r="G55"/>
     </row>
     <row r="56" spans="1:7" ht="15">
@@ -2721,7 +2741,7 @@
       <c r="E60" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="F60" s="51"/>
+      <c r="F60" s="47"/>
       <c r="G60"/>
     </row>
     <row r="61" spans="1:7" ht="15">
@@ -2741,7 +2761,7 @@
       <c r="E61" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="F61" s="51"/>
+      <c r="F61" s="47"/>
       <c r="G61"/>
     </row>
     <row r="62" spans="1:7" ht="15">
@@ -2761,7 +2781,7 @@
       <c r="E62" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="F62" s="51"/>
+      <c r="F62" s="47"/>
       <c r="G62"/>
     </row>
     <row r="63" spans="1:7" ht="15">
@@ -2781,7 +2801,7 @@
       <c r="E63" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="F63" s="51"/>
+      <c r="F63" s="47"/>
       <c r="G63"/>
     </row>
     <row r="64" spans="1:7" ht="34" customHeight="1">
@@ -2801,19 +2821,30 @@
       <c r="E64" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="F64" s="47"/>
+      <c r="F64" s="50"/>
       <c r="G64"/>
     </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="36"/>
-      <c r="B65" s="37"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="46"/>
-      <c r="F65" s="51"/>
+    <row r="65" spans="1:7" ht="15">
+      <c r="A65" s="36">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B65" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="E65" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="F65" s="47"/>
       <c r="G65"/>
     </row>
-    <row r="66" spans="1:7" ht="45" customHeight="1">
+    <row r="66" spans="1:7">
       <c r="A66" s="36"/>
       <c r="B66" s="37"/>
       <c r="C66" s="38"/>
@@ -2822,22 +2853,60 @@
       <c r="F66" s="47"/>
       <c r="G66"/>
     </row>
-    <row r="67" spans="1:7" ht="14" customHeight="1">
-      <c r="A67" s="20"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="42"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="58"/>
-      <c r="F67" s="59"/>
+    <row r="67" spans="1:7" ht="45" customHeight="1">
+      <c r="A67" s="36"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="50"/>
       <c r="G67"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" ht="14" customHeight="1">
+      <c r="A68" s="20"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="42"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="48"/>
+      <c r="F68" s="49"/>
       <c r="G68"/>
     </row>
+    <row r="69" spans="1:7">
+      <c r="G69"/>
+    </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="45">
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E39:F39"/>
     <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="E47:F47"/>
@@ -2852,38 +2921,10 @@
     <mergeCell ref="E62:F62"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E50:F50"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D81" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D82" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>